<commit_message>
*changed exportBad to exportLists, now sending all lists to logs and emptying lists after export *added log directory and files *added searchService function to select service, added function call to start of import options  On branch dev  Changes to be committed: 	modified:   dataframe.xlsx 	modified:   dbxls.xlsx 	modified:   log/bad_list 	modified:   log/dbIsbn_list 	modified:   log/dup_list 	modified:   log/isbn_list 	modified:   newMain.py 	new file:   scratch2.py 	modified:   scratchpad.py
</commit_message>
<xml_diff>
--- a/dbxls.xlsx
+++ b/dbxls.xlsx
@@ -14,9 +14,189 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="61">
   <si>
     <t>isbn</t>
+  </si>
+  <si>
+    <t>9780072263503</t>
+  </si>
+  <si>
+    <t>9780073517216</t>
+  </si>
+  <si>
+    <t>9780130206015</t>
+  </si>
+  <si>
+    <t>9780132360395</t>
+  </si>
+  <si>
+    <t>9780134000022</t>
+  </si>
+  <si>
+    <t>9780134277554</t>
+  </si>
+  <si>
+    <t>9780134496009</t>
+  </si>
+  <si>
+    <t>9780201563177</t>
+  </si>
+  <si>
+    <t>9780201835953</t>
+  </si>
+  <si>
+    <t>9780471168942</t>
+  </si>
+  <si>
+    <t>9780471946939</t>
+  </si>
+  <si>
+    <t>9780596000035</t>
+  </si>
+  <si>
+    <t>9780596000257</t>
+  </si>
+  <si>
+    <t>9780672311079</t>
+  </si>
+  <si>
+    <t>9780764548338</t>
+  </si>
+  <si>
+    <t>9780789735973</t>
+  </si>
+  <si>
+    <t>9780982131428</t>
+  </si>
+  <si>
+    <t>9781118983843</t>
+  </si>
+  <si>
+    <t>9781119572671</t>
+  </si>
+  <si>
+    <t>9781119722335</t>
+  </si>
+  <si>
+    <t>9781305880290</t>
+  </si>
+  <si>
+    <t>9781449305352</t>
+  </si>
+  <si>
+    <t>9781449316389</t>
+  </si>
+  <si>
+    <t>9781449357016</t>
+  </si>
+  <si>
+    <t>9781449387860</t>
+  </si>
+  <si>
+    <t>9781484269206</t>
+  </si>
+  <si>
+    <t>9781491924358</t>
+  </si>
+  <si>
+    <t>9781491927571</t>
+  </si>
+  <si>
+    <t>9781491929124</t>
+  </si>
+  <si>
+    <t>9781491931257</t>
+  </si>
+  <si>
+    <t>9781491979808</t>
+  </si>
+  <si>
+    <t>9781492040767</t>
+  </si>
+  <si>
+    <t>9781492057697</t>
+  </si>
+  <si>
+    <t>9781509300914</t>
+  </si>
+  <si>
+    <t>9781565924277</t>
+  </si>
+  <si>
+    <t>9781565924956</t>
+  </si>
+  <si>
+    <t>9781565927094</t>
+  </si>
+  <si>
+    <t>9781578700479</t>
+  </si>
+  <si>
+    <t>9781593272203</t>
+  </si>
+  <si>
+    <t>9781593273897</t>
+  </si>
+  <si>
+    <t>9781593279189</t>
+  </si>
+  <si>
+    <t>9781617293726</t>
+  </si>
+  <si>
+    <t>9781617294167</t>
+  </si>
+  <si>
+    <t>9781617294440</t>
+  </si>
+  <si>
+    <t>9781617295096</t>
+  </si>
+  <si>
+    <t>9781617295508</t>
+  </si>
+  <si>
+    <t>9781617295980</t>
+  </si>
+  <si>
+    <t>9781617296987</t>
+  </si>
+  <si>
+    <t>9781617297519</t>
+  </si>
+  <si>
+    <t>9781617297625</t>
+  </si>
+  <si>
+    <t>9781784390891</t>
+  </si>
+  <si>
+    <t>9781784399597</t>
+  </si>
+  <si>
+    <t>9781788990554</t>
+  </si>
+  <si>
+    <t>9781800564640</t>
+  </si>
+  <si>
+    <t>9781838552183</t>
+  </si>
+  <si>
+    <t>9781838820756</t>
+  </si>
+  <si>
+    <t>9781838981778</t>
+  </si>
+  <si>
+    <t>9781838983444</t>
+  </si>
+  <si>
+    <t>9781839214189</t>
+  </si>
+  <si>
+    <t>9798653385322</t>
   </si>
 </sst>
 </file>
@@ -374,15 +554,495 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B1"/>
+  <dimension ref="A1:B61"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="2:2">
+    <row r="1" spans="1:2">
       <c r="B1" s="1" t="s">
         <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" s="1">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" s="1">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" s="1">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" s="1">
+        <v>3</v>
+      </c>
+      <c r="B5" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" s="1">
+        <v>4</v>
+      </c>
+      <c r="B6" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7" s="1">
+        <v>5</v>
+      </c>
+      <c r="B7" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8" s="1">
+        <v>6</v>
+      </c>
+      <c r="B8" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9" s="1">
+        <v>7</v>
+      </c>
+      <c r="B9" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="A10" s="1">
+        <v>8</v>
+      </c>
+      <c r="B10" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2">
+      <c r="A11" s="1">
+        <v>9</v>
+      </c>
+      <c r="B11" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2">
+      <c r="A12" s="1">
+        <v>10</v>
+      </c>
+      <c r="B12" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2">
+      <c r="A13" s="1">
+        <v>11</v>
+      </c>
+      <c r="B13" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2">
+      <c r="A14" s="1">
+        <v>12</v>
+      </c>
+      <c r="B14" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2">
+      <c r="A15" s="1">
+        <v>13</v>
+      </c>
+      <c r="B15" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2">
+      <c r="A16" s="1">
+        <v>14</v>
+      </c>
+      <c r="B16" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2">
+      <c r="A17" s="1">
+        <v>15</v>
+      </c>
+      <c r="B17" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2">
+      <c r="A18" s="1">
+        <v>16</v>
+      </c>
+      <c r="B18" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2">
+      <c r="A19" s="1">
+        <v>17</v>
+      </c>
+      <c r="B19" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2">
+      <c r="A20" s="1">
+        <v>18</v>
+      </c>
+      <c r="B20" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2">
+      <c r="A21" s="1">
+        <v>19</v>
+      </c>
+      <c r="B21" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2">
+      <c r="A22" s="1">
+        <v>20</v>
+      </c>
+      <c r="B22" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2">
+      <c r="A23" s="1">
+        <v>21</v>
+      </c>
+      <c r="B23" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2">
+      <c r="A24" s="1">
+        <v>22</v>
+      </c>
+      <c r="B24" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2">
+      <c r="A25" s="1">
+        <v>23</v>
+      </c>
+      <c r="B25" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2">
+      <c r="A26" s="1">
+        <v>24</v>
+      </c>
+      <c r="B26" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2">
+      <c r="A27" s="1">
+        <v>25</v>
+      </c>
+      <c r="B27" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2">
+      <c r="A28" s="1">
+        <v>26</v>
+      </c>
+      <c r="B28" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2">
+      <c r="A29" s="1">
+        <v>27</v>
+      </c>
+      <c r="B29" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2">
+      <c r="A30" s="1">
+        <v>28</v>
+      </c>
+      <c r="B30" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2">
+      <c r="A31" s="1">
+        <v>29</v>
+      </c>
+      <c r="B31" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2">
+      <c r="A32" s="1">
+        <v>30</v>
+      </c>
+      <c r="B32" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2">
+      <c r="A33" s="1">
+        <v>31</v>
+      </c>
+      <c r="B33" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2">
+      <c r="A34" s="1">
+        <v>32</v>
+      </c>
+      <c r="B34" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2">
+      <c r="A35" s="1">
+        <v>33</v>
+      </c>
+      <c r="B35" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2">
+      <c r="A36" s="1">
+        <v>34</v>
+      </c>
+      <c r="B36" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2">
+      <c r="A37" s="1">
+        <v>35</v>
+      </c>
+      <c r="B37" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2">
+      <c r="A38" s="1">
+        <v>36</v>
+      </c>
+      <c r="B38" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2">
+      <c r="A39" s="1">
+        <v>37</v>
+      </c>
+      <c r="B39" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2">
+      <c r="A40" s="1">
+        <v>38</v>
+      </c>
+      <c r="B40" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2">
+      <c r="A41" s="1">
+        <v>39</v>
+      </c>
+      <c r="B41" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2">
+      <c r="A42" s="1">
+        <v>40</v>
+      </c>
+      <c r="B42" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2">
+      <c r="A43" s="1">
+        <v>41</v>
+      </c>
+      <c r="B43" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2">
+      <c r="A44" s="1">
+        <v>42</v>
+      </c>
+      <c r="B44" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2">
+      <c r="A45" s="1">
+        <v>43</v>
+      </c>
+      <c r="B45" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2">
+      <c r="A46" s="1">
+        <v>44</v>
+      </c>
+      <c r="B46" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2">
+      <c r="A47" s="1">
+        <v>45</v>
+      </c>
+      <c r="B47" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2">
+      <c r="A48" s="1">
+        <v>46</v>
+      </c>
+      <c r="B48" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2">
+      <c r="A49" s="1">
+        <v>47</v>
+      </c>
+      <c r="B49" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2">
+      <c r="A50" s="1">
+        <v>48</v>
+      </c>
+      <c r="B50" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2">
+      <c r="A51" s="1">
+        <v>49</v>
+      </c>
+      <c r="B51" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2">
+      <c r="A52" s="1">
+        <v>50</v>
+      </c>
+      <c r="B52" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2">
+      <c r="A53" s="1">
+        <v>51</v>
+      </c>
+      <c r="B53" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2">
+      <c r="A54" s="1">
+        <v>52</v>
+      </c>
+      <c r="B54" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2">
+      <c r="A55" s="1">
+        <v>53</v>
+      </c>
+      <c r="B55" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2">
+      <c r="A56" s="1">
+        <v>54</v>
+      </c>
+      <c r="B56" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2">
+      <c r="A57" s="1">
+        <v>55</v>
+      </c>
+      <c r="B57" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2">
+      <c r="A58" s="1">
+        <v>56</v>
+      </c>
+      <c r="B58" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2">
+      <c r="A59" s="1">
+        <v>57</v>
+      </c>
+      <c r="B59" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2">
+      <c r="A60" s="1">
+        <v>58</v>
+      </c>
+      <c r="B60" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2">
+      <c r="A61" s="1">
+        <v>59</v>
+      </c>
+      <c r="B61" t="s">
+        <v>60</v>
       </c>
     </row>
   </sheetData>

</xml_diff>